<commit_message>
add more source files (1990-2017)
</commit_message>
<xml_diff>
--- a/etl/source/CPI 2015_data.xlsx
+++ b/etl/source/CPI 2015_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\ER-Group\Communications\1.Projects\CPI\2015\Website and blog\Downloads\Data &amp; methodology\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27045" windowHeight="13515"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24600" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="CPI 2015" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'CPI 2015'!$A$1:$AA$170</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'CPI 2015'!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1207,10 +1207,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1807,7 +1807,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1842,7 +1842,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2019,7 +2019,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2027,30 +2027,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F179" sqref="F179"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R100" sqref="R100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="10.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="9" customWidth="1"/>
-    <col min="20" max="26" width="8.7109375" customWidth="1"/>
-    <col min="27" max="28" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="9"/>
+    <col min="2" max="2" width="10.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="9" customWidth="1"/>
+    <col min="20" max="26" width="8.6640625" customWidth="1"/>
+    <col min="27" max="28" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:27" ht="46.5" customHeight="1">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2065,7 +2065,7 @@
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
     </row>
-    <row r="2" spans="1:27" s="7" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="7" customFormat="1" ht="100" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>333</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="8">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S6" s="9">
         <v>4</v>
@@ -2438,17 +2438,17 @@
       </c>
       <c r="Y6" s="4">
         <f t="shared" si="0"/>
-        <v>84.0565</v>
+        <v>87.0565</v>
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="1"/>
-        <v>91.9435</v>
+        <v>94.9435</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="8">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="S7" s="9">
         <v>5</v>
@@ -2513,17 +2513,17 @@
       </c>
       <c r="Y7" s="4">
         <f t="shared" si="0"/>
-        <v>84.013499999999993</v>
+        <v>81.013499999999993</v>
       </c>
       <c r="Z7" s="4">
         <f t="shared" si="1"/>
-        <v>89.986500000000007</v>
+        <v>86.986500000000007</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="8">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S8" s="9">
         <v>5</v>
@@ -2588,17 +2588,17 @@
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="0"/>
-        <v>82.05</v>
+        <v>83.05</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" si="1"/>
-        <v>91.95</v>
+        <v>92.95</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="8">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S13" s="9">
         <v>10</v>
@@ -2959,17 +2959,17 @@
       </c>
       <c r="Y13" s="4">
         <f>(R13-1.65*V13)</f>
-        <v>71.067000000000007</v>
+        <v>75.067000000000007</v>
       </c>
       <c r="Z13" s="4">
         <f>(R13+1.65*V13)</f>
-        <v>90.932999999999993</v>
+        <v>94.932999999999993</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27">
       <c r="A14" s="9">
         <v>10</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27">
       <c r="A15" s="9">
         <v>13</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27">
       <c r="A17" s="9">
         <v>15</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27">
       <c r="A18" s="9">
         <v>16</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27">
       <c r="A20" s="9">
         <v>18</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27">
       <c r="A23" s="9">
         <v>21</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27">
       <c r="A24" s="9">
         <v>22</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27">
       <c r="A25" s="9">
         <v>23</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27">
       <c r="A28" s="9">
         <v>23</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27">
       <c r="A29" s="9">
         <v>27</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27">
       <c r="A30" s="9">
         <v>28</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -4281,7 +4281,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="8">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S31" s="9">
         <v>28</v>
@@ -4303,17 +4303,17 @@
       </c>
       <c r="Y31" s="4">
         <f t="shared" si="0"/>
-        <v>58.561500000000002</v>
+        <v>59.561500000000002</v>
       </c>
       <c r="Z31" s="4">
         <f t="shared" si="1"/>
-        <v>67.438500000000005</v>
+        <v>68.438500000000005</v>
       </c>
       <c r="AA31" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27">
       <c r="A32" s="9">
         <v>30</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>55</v>
       </c>
       <c r="R32" s="8">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="S32" s="9">
         <v>30</v>
@@ -4382,17 +4382,17 @@
       </c>
       <c r="Y32" s="4">
         <f t="shared" si="0"/>
-        <v>58.188499999999998</v>
+        <v>59.188499999999998</v>
       </c>
       <c r="Z32" s="4">
         <f t="shared" si="1"/>
-        <v>65.811499999999995</v>
+        <v>66.811499999999995</v>
       </c>
       <c r="AA32" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27">
       <c r="A34" s="9">
         <v>32</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27">
       <c r="A35" s="9">
         <v>32</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27">
       <c r="A36" s="9">
         <v>32</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>55</v>
       </c>
       <c r="R36" s="8">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S36" s="9">
         <v>32</v>
@@ -4678,17 +4678,17 @@
       </c>
       <c r="Y36" s="4">
         <f t="shared" si="2"/>
-        <v>55.521999999999998</v>
+        <v>53.521999999999998</v>
       </c>
       <c r="Z36" s="4">
         <f t="shared" si="3"/>
-        <v>66.477999999999994</v>
+        <v>64.477999999999994</v>
       </c>
       <c r="AA36" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27">
       <c r="A37" s="9">
         <v>35</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27">
       <c r="A38" s="9">
         <v>36</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27">
       <c r="A39" s="9">
         <v>37</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27">
       <c r="A40" s="9">
         <v>37</v>
       </c>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="8">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S40" s="9">
         <v>37</v>
@@ -4990,17 +4990,17 @@
       </c>
       <c r="Y40" s="4">
         <f t="shared" si="2"/>
-        <v>50.901499999999999</v>
+        <v>48.901499999999999</v>
       </c>
       <c r="Z40" s="4">
         <f t="shared" si="3"/>
-        <v>61.098500000000001</v>
+        <v>59.098500000000001</v>
       </c>
       <c r="AA40" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27">
       <c r="A41" s="9">
         <v>37</v>
       </c>
@@ -5037,7 +5037,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="8">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="S41" s="9">
         <v>37</v>
@@ -5059,17 +5059,17 @@
       </c>
       <c r="Y41" s="4">
         <f t="shared" si="2"/>
-        <v>47.849000000000004</v>
+        <v>51.849000000000004</v>
       </c>
       <c r="Z41" s="4">
         <f t="shared" si="3"/>
-        <v>64.150999999999996</v>
+        <v>68.150999999999996</v>
       </c>
       <c r="AA41" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27">
       <c r="A42" s="9">
         <v>40</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27">
       <c r="A43" s="9">
         <v>40</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27">
       <c r="A44" s="9">
         <v>40</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>60</v>
       </c>
       <c r="R44" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S44" s="9">
         <v>40</v>
@@ -5278,17 +5278,17 @@
       </c>
       <c r="Y44" s="4">
         <f t="shared" si="2"/>
-        <v>51.749499999999998</v>
+        <v>52.749499999999998</v>
       </c>
       <c r="Z44" s="4">
         <f t="shared" si="3"/>
-        <v>58.250500000000002</v>
+        <v>59.250500000000002</v>
       </c>
       <c r="AA44" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27">
       <c r="A45" s="9">
         <v>40</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27">
       <c r="A46" s="9">
         <v>44</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27">
       <c r="A47" s="9">
         <v>45</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27">
       <c r="A48" s="9">
         <v>45</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27">
       <c r="A49" s="9">
         <v>45</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27">
       <c r="A50" s="9">
         <v>48</v>
       </c>
@@ -5712,7 +5712,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27">
       <c r="A51" s="9">
         <v>48</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27">
       <c r="A52" s="9">
         <v>50</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27">
       <c r="A53" s="9">
         <v>50</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27">
       <c r="A54" s="9">
         <v>50</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27">
       <c r="A55" s="9">
         <v>50</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27">
       <c r="A56" s="9">
         <v>54</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27">
       <c r="A57" s="9">
         <v>55</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27">
       <c r="A58" s="9">
         <v>56</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27">
       <c r="A59" s="9">
         <v>56</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27">
       <c r="A60" s="9">
         <v>58</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27">
       <c r="A61" s="9">
         <v>58</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27">
       <c r="A62" s="9">
         <v>60</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27">
       <c r="A63" s="9">
         <v>61</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27">
       <c r="A64" s="9">
         <v>61</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27">
       <c r="A65" s="9">
         <v>61</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27">
       <c r="A66" s="9">
         <v>61</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27">
       <c r="A67" s="9">
         <v>61</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27">
       <c r="A68" s="9">
         <v>66</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27">
       <c r="A69" s="9">
         <v>66</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27">
       <c r="A70" s="9">
         <v>66</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27">
       <c r="A71" s="9">
         <v>69</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27">
       <c r="A72" s="9">
         <v>69</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27">
       <c r="A73" s="9">
         <v>71</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27">
       <c r="A74" s="9">
         <v>72</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27">
       <c r="A75" s="9">
         <v>72</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27">
       <c r="A76" s="9">
         <v>72</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27">
       <c r="A77" s="9">
         <v>72</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27">
       <c r="A78" s="9">
         <v>76</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27">
       <c r="A79" s="9">
         <v>76</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27">
       <c r="A80" s="9">
         <v>76</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27">
       <c r="A81" s="9">
         <v>76</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27">
       <c r="A82" s="9">
         <v>76</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27">
       <c r="A83" s="9">
         <v>76</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27">
       <c r="A84" s="9">
         <v>76</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27">
       <c r="A85" s="9">
         <v>83</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27">
       <c r="A86" s="9">
         <v>83</v>
       </c>
@@ -8386,7 +8386,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27">
       <c r="A87" s="9">
         <v>83</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27">
       <c r="A88" s="9">
         <v>83</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27">
       <c r="A89" s="9">
         <v>83</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27">
       <c r="A90" s="9">
         <v>88</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27">
       <c r="A91" s="9">
         <v>88</v>
       </c>
@@ -8757,7 +8757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27">
       <c r="A92" s="9">
         <v>88</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27">
       <c r="A93" s="9">
         <v>88</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27">
       <c r="A94" s="9">
         <v>88</v>
       </c>
@@ -8980,7 +8980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27">
       <c r="A95" s="9">
         <v>88</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27">
       <c r="A96" s="9">
         <v>88</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27">
       <c r="A97" s="9">
         <v>95</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27">
       <c r="A98" s="9">
         <v>95</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27">
       <c r="A99" s="9">
         <v>95</v>
       </c>
@@ -9311,7 +9311,7 @@
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
       <c r="R99" s="8">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S99" s="9">
         <v>95</v>
@@ -9333,17 +9333,17 @@
       </c>
       <c r="Y99" s="4">
         <f t="shared" si="4"/>
-        <v>25.083500000000001</v>
+        <v>21.083500000000001</v>
       </c>
       <c r="Z99" s="4">
         <f t="shared" si="5"/>
-        <v>44.916499999999999</v>
+        <v>40.916499999999999</v>
       </c>
       <c r="AA99" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27">
       <c r="A100" s="9">
         <v>95</v>
       </c>
@@ -9420,7 +9420,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27">
       <c r="A101" s="9">
         <v>99</v>
       </c>
@@ -9495,7 +9495,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27">
       <c r="A102" s="9">
         <v>99</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27">
       <c r="A103" s="9">
         <v>99</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27">
       <c r="A104" s="9">
         <v>99</v>
       </c>
@@ -9702,7 +9702,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27">
       <c r="A105" s="9">
         <v>103</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27">
       <c r="A106" s="9">
         <v>103</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27">
       <c r="A107" s="9">
         <v>103</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27">
       <c r="A108" s="9">
         <v>103</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27">
       <c r="A109" s="9">
         <v>107</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27">
       <c r="A110" s="9">
         <v>107</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27">
       <c r="A111" s="9">
         <v>107</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27">
       <c r="A112" s="9">
         <v>107</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27">
       <c r="A113" s="9">
         <v>107</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27">
       <c r="A114" s="9">
         <v>112</v>
       </c>
@@ -10440,7 +10440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27">
       <c r="A115" s="9">
         <v>112</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27">
       <c r="A116" s="9">
         <v>112</v>
       </c>
@@ -10588,7 +10588,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27">
       <c r="A117" s="9">
         <v>112</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27">
       <c r="A118" s="9">
         <v>112</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27">
       <c r="A119" s="9">
         <v>117</v>
       </c>
@@ -10815,7 +10815,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27">
       <c r="A120" s="9">
         <v>117</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27">
       <c r="A121" s="9">
         <v>119</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27">
       <c r="A122" s="9">
         <v>119</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27">
       <c r="A123" s="9">
         <v>119</v>
       </c>
@@ -11111,7 +11111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27">
       <c r="A124" s="9">
         <v>119</v>
       </c>
@@ -11188,7 +11188,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27">
       <c r="A125" s="9">
         <v>123</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27">
       <c r="A126" s="9">
         <v>123</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27">
       <c r="A127" s="9">
         <v>123</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27">
       <c r="A128" s="9">
         <v>123</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27">
       <c r="A129" s="9">
         <v>123</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27">
       <c r="A130" s="9">
         <v>123</v>
       </c>
@@ -11630,7 +11630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27">
       <c r="A131" s="9">
         <v>123</v>
       </c>
@@ -11697,7 +11697,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27">
       <c r="A132" s="9">
         <v>130</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27">
       <c r="A133" s="9">
         <v>130</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27">
       <c r="A134" s="9">
         <v>130</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27">
       <c r="A135" s="9">
         <v>130</v>
       </c>
@@ -11993,7 +11993,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27">
       <c r="A136" s="9">
         <v>130</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:27">
       <c r="A137" s="9">
         <v>130</v>
       </c>
@@ -12141,7 +12141,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:27">
       <c r="A138" s="9">
         <v>136</v>
       </c>
@@ -12208,7 +12208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:27">
       <c r="A139" s="9">
         <v>136</v>
       </c>
@@ -12285,7 +12285,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:27">
       <c r="A140" s="9">
         <v>136</v>
       </c>
@@ -12356,7 +12356,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:27">
       <c r="A141" s="9">
         <v>139</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27">
       <c r="A142" s="9">
         <v>139</v>
       </c>
@@ -12504,7 +12504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:27">
       <c r="A143" s="9">
         <v>139</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:27">
       <c r="A144" s="9">
         <v>139</v>
       </c>
@@ -12650,7 +12650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:27">
       <c r="A145" s="9">
         <v>139</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:27">
       <c r="A146" s="9">
         <v>139</v>
       </c>
@@ -12798,7 +12798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:27">
       <c r="A147" s="9">
         <v>145</v>
       </c>
@@ -12867,7 +12867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:27">
       <c r="A148" s="9">
         <v>146</v>
       </c>
@@ -12940,7 +12940,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:27">
       <c r="A149" s="9">
         <v>147</v>
       </c>
@@ -13011,7 +13011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:27">
       <c r="A150" s="9">
         <v>147</v>
       </c>
@@ -13084,7 +13084,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:27">
       <c r="A151" s="9">
         <v>147</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:27">
       <c r="A152" s="9">
         <v>150</v>
       </c>
@@ -13230,7 +13230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:27">
       <c r="A153" s="9">
         <v>150</v>
       </c>
@@ -13305,7 +13305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:27">
       <c r="A154" s="9">
         <v>150</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:27">
       <c r="A155" s="9">
         <v>153</v>
       </c>
@@ -13455,7 +13455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:27">
       <c r="A156" s="9">
         <v>154</v>
       </c>
@@ -13524,7 +13524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:27">
       <c r="A157" s="9">
         <v>154</v>
       </c>
@@ -13593,7 +13593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:27">
       <c r="A158" s="9">
         <v>154</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:27">
       <c r="A159" s="9">
         <v>154</v>
       </c>
@@ -13735,7 +13735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:27">
       <c r="A160" s="9">
         <v>158</v>
       </c>
@@ -13806,7 +13806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:27">
       <c r="A161" s="9">
         <v>158</v>
       </c>
@@ -13875,7 +13875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:27">
       <c r="A162" s="9">
         <v>158</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:27">
       <c r="A163" s="9">
         <v>161</v>
       </c>
@@ -14019,7 +14019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:27">
       <c r="A164" s="9">
         <v>161</v>
       </c>
@@ -14090,7 +14090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:27">
       <c r="A165" s="9">
         <v>163</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:27">
       <c r="A166" s="9">
         <v>163</v>
       </c>
@@ -14228,7 +14228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:27">
       <c r="A167" s="9">
         <v>165</v>
       </c>
@@ -14301,7 +14301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:27">
       <c r="A168" s="9">
         <v>166</v>
       </c>
@@ -14370,7 +14370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:27">
       <c r="A169" s="9">
         <v>167</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:27">
       <c r="A170" s="9">
         <v>167</v>
       </c>
@@ -14506,11 +14506,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:27">
       <c r="H171" s="4"/>
       <c r="J171" s="1"/>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:27">
       <c r="J172" s="1"/>
       <c r="V172" s="10"/>
     </row>
@@ -14521,12 +14521,17 @@
   </sortState>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="67" fitToHeight="0" orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;F</oddHeader>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>